<commit_message>
Talk together about the diagramm corrections (not added to the document now only in VP) and discuss the java project
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3+4_team_3_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3+4_team_3_lernjournal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37200" yWindow="960" windowWidth="28760" windowHeight="19680" tabRatio="415" activeTab="1"/>
+    <workbookView xWindow="38060" yWindow="880" windowWidth="29180" windowHeight="19920" tabRatio="415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -166,6 +166,25 @@
   </si>
   <si>
     <t>11.11.13</t>
+  </si>
+  <si>
+    <t>14.11.13</t>
+  </si>
+  <si>
+    <t>8-9.11.13</t>
+  </si>
+  <si>
+    <t>16.11.13</t>
+  </si>
+  <si>
+    <t>Besprechung Korrekturen Diagramm.
+Implementation zusammentragen und umsetzten.</t>
+  </si>
+  <si>
+    <t>Erste gedanken und umsetztung der Implementation</t>
+  </si>
+  <si>
+    <t>Diagramm Korrekturen, vortsetztung implementation</t>
   </si>
 </sst>
 </file>
@@ -227,7 +246,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -343,8 +362,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -454,8 +493,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -517,33 +564,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -589,8 +630,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="117">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -645,6 +716,10 @@
     <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -699,6 +774,10 @@
     <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1061,11 +1140,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1237,13 +1316,13 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" s="11" customFormat="1">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="26">
         <v>45</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="27">
         <v>41434</v>
       </c>
       <c r="D11" s="10"/>
@@ -1261,13 +1340,13 @@
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" s="11" customFormat="1">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="26">
         <v>5</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="27">
         <v>41434</v>
       </c>
       <c r="D12" s="10"/>
@@ -1285,13 +1364,13 @@
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:16" s="11" customFormat="1">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="26">
         <v>45</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="27">
         <v>41434</v>
       </c>
       <c r="D13" s="10"/>
@@ -1309,13 +1388,13 @@
       <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="23">
         <v>30</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="24">
         <v>41436</v>
       </c>
       <c r="D14" s="10"/>
@@ -1333,13 +1412,13 @@
       <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="31">
         <v>105</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="32">
         <v>41441</v>
       </c>
       <c r="D15" s="10"/>
@@ -1357,13 +1436,13 @@
       <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="34">
         <v>35</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="35">
         <v>41538</v>
       </c>
       <c r="D16" s="10"/>
@@ -1381,13 +1460,13 @@
       <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="26">
         <v>65</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="27">
         <v>41538</v>
       </c>
       <c r="D17" s="10"/>
@@ -1405,13 +1484,13 @@
       <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="26">
         <v>20</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="27">
         <v>41538</v>
       </c>
       <c r="D18" s="10"/>
@@ -1429,13 +1508,13 @@
       <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="39">
+      <c r="B19" s="37">
         <v>45</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="38">
         <v>41545</v>
       </c>
       <c r="D19" s="10"/>
@@ -1453,13 +1532,13 @@
       <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="40">
         <v>30</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="41">
         <v>41552</v>
       </c>
       <c r="D20" s="10"/>
@@ -1477,13 +1556,13 @@
       <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16" s="11" customFormat="1">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="26">
         <v>60</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="27">
         <v>41553</v>
       </c>
       <c r="D21" s="10"/>
@@ -1501,9 +1580,9 @@
       <c r="P21" s="10"/>
     </row>
     <row r="22" spans="1:16" s="11" customFormat="1">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1681,13 +1760,13 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" s="11" customFormat="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="23">
+      <c r="B31" s="21">
         <v>20</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="22">
         <v>41433</v>
       </c>
       <c r="D31" s="10"/>
@@ -1705,13 +1784,13 @@
       <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:16" s="11" customFormat="1">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="26">
         <v>25</v>
       </c>
-      <c r="C32" s="29">
+      <c r="C32" s="27">
         <v>41434</v>
       </c>
       <c r="D32" s="10"/>
@@ -1729,13 +1808,13 @@
       <c r="P32" s="10"/>
     </row>
     <row r="33" spans="1:16" s="11" customFormat="1">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="28">
+      <c r="B33" s="26">
         <v>50</v>
       </c>
-      <c r="C33" s="29">
+      <c r="C33" s="27">
         <v>41440</v>
       </c>
       <c r="D33" s="10"/>
@@ -1753,13 +1832,13 @@
       <c r="P33" s="10"/>
     </row>
     <row r="34" spans="1:16" s="11" customFormat="1">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="28">
+      <c r="B34" s="26">
         <v>15</v>
       </c>
-      <c r="C34" s="29">
+      <c r="C34" s="27">
         <v>41439</v>
       </c>
       <c r="D34" s="10"/>
@@ -1777,13 +1856,13 @@
       <c r="P34" s="10"/>
     </row>
     <row r="35" spans="1:16" s="11" customFormat="1" ht="37" thickBot="1">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="33">
+      <c r="B35" s="31">
         <v>105</v>
       </c>
-      <c r="C35" s="34">
+      <c r="C35" s="32">
         <v>41441</v>
       </c>
       <c r="D35" s="10"/>
@@ -1801,13 +1880,13 @@
       <c r="P35" s="10"/>
     </row>
     <row r="36" spans="1:16" s="11" customFormat="1" ht="25" thickTop="1">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="36">
+      <c r="B36" s="34">
         <v>35</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="35">
         <v>41535</v>
       </c>
       <c r="D36" s="10"/>
@@ -1825,13 +1904,13 @@
       <c r="P36" s="10"/>
     </row>
     <row r="37" spans="1:16" s="11" customFormat="1">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="28">
+      <c r="B37" s="26">
         <v>35</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37" s="27">
         <v>41538</v>
       </c>
       <c r="D37" s="10"/>
@@ -1849,13 +1928,13 @@
       <c r="P37" s="10"/>
     </row>
     <row r="38" spans="1:16" s="11" customFormat="1">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="26">
         <v>65</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38" s="27">
         <v>41538</v>
       </c>
       <c r="D38" s="10"/>
@@ -1873,13 +1952,13 @@
       <c r="P38" s="10"/>
     </row>
     <row r="39" spans="1:16" s="11" customFormat="1">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="28">
+      <c r="B39" s="26">
         <v>20</v>
       </c>
-      <c r="C39" s="29">
+      <c r="C39" s="27">
         <v>41538</v>
       </c>
       <c r="D39" s="10"/>
@@ -1897,13 +1976,13 @@
       <c r="P39" s="10"/>
     </row>
     <row r="40" spans="1:16" s="11" customFormat="1">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="28">
+      <c r="B40" s="26">
         <v>15</v>
       </c>
-      <c r="C40" s="30">
+      <c r="C40" s="28">
         <v>41538</v>
       </c>
       <c r="D40" s="10"/>
@@ -1921,13 +2000,13 @@
       <c r="P40" s="10"/>
     </row>
     <row r="41" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="39">
+      <c r="B41" s="37">
         <v>45</v>
       </c>
-      <c r="C41" s="40">
+      <c r="C41" s="38">
         <v>41545</v>
       </c>
       <c r="D41" s="10"/>
@@ -1945,13 +2024,13 @@
       <c r="P41" s="10"/>
     </row>
     <row r="42" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="28">
+      <c r="B42" s="26">
         <v>60</v>
       </c>
-      <c r="C42" s="29">
+      <c r="C42" s="27">
         <v>41553</v>
       </c>
       <c r="D42" s="10"/>
@@ -2292,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2325,11 +2404,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2402,8 +2481,8 @@
     </row>
     <row r="6" spans="1:16" s="4" customFormat="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -2460,8 +2539,8 @@
     </row>
     <row r="9" spans="1:16" s="4" customFormat="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -2501,13 +2580,13 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" s="11" customFormat="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="26">
         <v>60</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="10"/>
@@ -2524,14 +2603,14 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+      <c r="A12" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="43">
         <v>60</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="44" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="10"/>
@@ -2548,10 +2627,10 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+      <c r="A13" s="45"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -2566,10 +2645,14 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1">
-      <c r="A14" s="20"/>
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A14" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -2602,10 +2685,10 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="12"/>
+    <row r="16" spans="1:16" s="11" customFormat="1">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -2620,93 +2703,89 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:16" s="4" customFormat="1">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:16" s="11" customFormat="1">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" s="4" customFormat="1">
+      <c r="A21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="18">
-        <f>SUM(B11:B16)</f>
+      <c r="B21" s="18">
+        <f>SUM(B11:B20)</f>
         <v>120</v>
       </c>
-      <c r="C17" s="19">
-        <f>TIME(0,B17,)</f>
+      <c r="C21" s="19">
+        <f>TIME(0,B21,)</f>
         <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" s="4" customFormat="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" s="4" customFormat="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" s="4" customFormat="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2741,15 +2820,9 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" s="4" customFormat="1">
-      <c r="A23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2764,111 +2837,97 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" s="11" customFormat="1">
-      <c r="A24" s="25" t="s">
+    <row r="24" spans="1:16" s="4" customFormat="1">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" s="4" customFormat="1">
+      <c r="A26" s="2"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" s="4" customFormat="1">
+      <c r="A27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" s="11" customFormat="1">
+      <c r="A28" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B28" s="26">
         <v>20</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C28" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-    </row>
-    <row r="25" spans="1:16" s="11" customFormat="1" ht="24">
-      <c r="A25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="28">
-        <v>90</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-    </row>
-    <row r="26" spans="1:16" s="11" customFormat="1">
-      <c r="A26" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="28">
-        <v>20</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-    </row>
-    <row r="27" spans="1:16" s="11" customFormat="1">
-      <c r="A27" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="28">
-        <v>60</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-    </row>
-    <row r="28" spans="1:16" s="11" customFormat="1">
-      <c r="A28" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="28">
-        <v>60</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>40</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -2884,10 +2943,16 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1">
-      <c r="A29" s="25"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="30"/>
+    <row r="29" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A29" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="26">
+        <v>90</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -2903,9 +2968,15 @@
       <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16" s="11" customFormat="1">
-      <c r="A30" s="25"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="30"/>
+      <c r="A30" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="26">
+        <v>20</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -2921,9 +2992,15 @@
       <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:16" s="11" customFormat="1">
-      <c r="A31" s="25"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="30"/>
+      <c r="A31" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="26">
+        <v>60</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -2938,10 +3015,16 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="12"/>
+    <row r="32" spans="1:16" s="11" customFormat="1" ht="13" thickBot="1">
+      <c r="A32" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="43">
+        <v>60</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -2956,160 +3039,152 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" s="4" customFormat="1">
-      <c r="A33" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="18">
-        <f>SUM(B24:B32)</f>
-        <v>250</v>
-      </c>
-      <c r="C33" s="19">
-        <f>TIME(0,B33,)</f>
-        <v>0.17361111111111113</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="1:16" s="4" customFormat="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-    </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-    </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
-      <c r="A37" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A39" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-    </row>
-    <row r="40" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="8">
-        <v>0</v>
-      </c>
-      <c r="C40" s="9">
-        <v>41275</v>
-      </c>
+    <row r="33" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
+      <c r="A33" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="34">
+        <v>40</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" s="11" customFormat="1">
+      <c r="A34" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="26">
+        <v>80</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+    </row>
+    <row r="35" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A35" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" s="11" customFormat="1">
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" s="11" customFormat="1">
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+    </row>
+    <row r="38" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A40" s="47"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -3124,56 +3199,53 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
-      <c r="A41" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="8">
-        <v>0</v>
-      </c>
-      <c r="C41" s="9">
-        <v>41275</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-    </row>
-    <row r="42" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
+    <row r="41" spans="1:16" s="4" customFormat="1">
+      <c r="A41" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="18">
+        <f>SUM(B28:B39)</f>
+        <v>370</v>
+      </c>
+      <c r="C41" s="19">
+        <f>TIME(0,B41,)</f>
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:16" s="4" customFormat="1">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" s="4" customFormat="1" hidden="1">
-      <c r="A43" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="14">
-        <f>SUM(B40:B42)</f>
-        <v>0</v>
-      </c>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="3"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -3189,17 +3261,31 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
     </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
-      <c r="A45" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="16">
-        <f>SUM(B33,B17)</f>
-        <v>370</v>
-      </c>
-      <c r="C45" s="17">
-        <f>TIME(0,B45,)</f>
-        <v>0.25694444444444448</v>
+    <row r="44" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="1:16" s="4" customFormat="1" ht="15" hidden="1">
+      <c r="A45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -3214,6 +3300,163 @@
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
+    </row>
+    <row r="46" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+    </row>
+    <row r="47" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+    </row>
+    <row r="48" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="8">
+        <v>0</v>
+      </c>
+      <c r="C48" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+    </row>
+    <row r="49" spans="1:16" s="11" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+      <c r="A49" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="8">
+        <v>0</v>
+      </c>
+      <c r="C49" s="9">
+        <v>41275</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+    </row>
+    <row r="50" spans="1:16" s="11" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+    </row>
+    <row r="51" spans="1:16" s="4" customFormat="1" hidden="1">
+      <c r="A51" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="14">
+        <f>SUM(B48:B50)</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+    </row>
+    <row r="53" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1">
+      <c r="A53" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="16">
+        <f>SUM(B41,B21)</f>
+        <v>490</v>
+      </c>
+      <c r="C53" s="17">
+        <f>TIME(0,B53,)</f>
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3271,11 +3514,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>

</xml_diff>